<commit_message>
DataDriven Commit for login
</commit_message>
<xml_diff>
--- a/ExcelSheets/TestData.xlsx
+++ b/ExcelSheets/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15300" windowHeight="6615"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16665" windowHeight="6615"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,13 @@
     <t>Password</t>
   </si>
   <si>
+    <t>demo</t>
+  </si>
+  <si>
     <t>demo1</t>
   </si>
   <si>
-    <t>demo2</t>
-  </si>
-  <si>
-    <t>demo3</t>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -55,12 +55,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -69,9 +84,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,38 +397,41 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B4" s="1">
         <v>1234</v>
       </c>
+      <c r="C4" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3456</v>
-      </c>
-    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>